<commit_message>
added ToInitialize.m % This file performs search and replace for all files inside % codegen/lib/fsdaC % The indication of the files is in the first column of Excel file named % ToInitialize.xlsx (a missing entry in the first column means consider all % files which have .c extension) % String to search is in the second column of Excel file % String to replace is in the third column of Excel file % Remark: this file must be run before copyFilesIntoDocuments.m
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4240188-BF5E-43FE-B77F-3A24496FFDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B29C10A-004C-4CD1-B6E4-D28C0746DC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>int j_loop_ub</t>
   </si>
   <si>
-    <t>int jloop_ub=0</t>
-  </si>
-  <si>
     <t xml:space="preserve">LTSts_wrapper.c   </t>
   </si>
   <si>
@@ -84,16 +81,19 @@
     <t>int i3=0</t>
   </si>
   <si>
+    <t>fflush(stdout);</t>
+  </si>
+  <si>
+    <t>//fflush(stdout);</t>
+  </si>
+  <si>
+    <t>int j_loop_ub=0</t>
+  </si>
+  <si>
     <t>printf(</t>
   </si>
   <si>
     <t>Rprintf(</t>
-  </si>
-  <si>
-    <t>fflush(stdout);</t>
-  </si>
-  <si>
-    <t>//fflush(stdout);</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,13 +460,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -488,56 +488,56 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added search and replace for (almost all) tclust files
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B29C10A-004C-4CD1-B6E4-D28C0746DC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AED23EC-FFA4-4BB6-9BA6-9FE262E0D26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>FSRcore.c</t>
   </si>
@@ -94,16 +94,64 @@
   </si>
   <si>
     <t>Rprintf(</t>
+  </si>
+  <si>
+    <t>tclust_wrapper.c</t>
+  </si>
+  <si>
+    <t>int i5</t>
+  </si>
+  <si>
+    <t>int i5=0</t>
+  </si>
+  <si>
+    <t>int i2</t>
+  </si>
+  <si>
+    <t>int i2=0</t>
+  </si>
+  <si>
+    <t>int e_loop_ub</t>
+  </si>
+  <si>
+    <t>int e_loop_ub=0</t>
+  </si>
+  <si>
+    <t>int d_loop_ub</t>
+  </si>
+  <si>
+    <t>int d_loop_ub=0</t>
+  </si>
+  <si>
+    <t>int b_loop_ub</t>
+  </si>
+  <si>
+    <t>int b_loop_ub=0</t>
+  </si>
+  <si>
+    <t>int c_loop_ub</t>
+  </si>
+  <si>
+    <t>int c_loop_ub=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tclust_wrapper1.c   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -445,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,22 +573,177 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C22" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
In file ToInitialize.xlsx Replaced in second column fflush(stdout); with fflush(stdout
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AED23EC-FFA4-4BB6-9BA6-9FE262E0D26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFE36F0-5014-4E69-9F27-502DB6B502A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -81,12 +81,6 @@
     <t>int i3=0</t>
   </si>
   <si>
-    <t>fflush(stdout);</t>
-  </si>
-  <si>
-    <t>//fflush(stdout);</t>
-  </si>
-  <si>
     <t>int j_loop_ub=0</t>
   </si>
   <si>
@@ -136,6 +130,12 @@
   </si>
   <si>
     <t xml:space="preserve">tclust_wrapper1.c   </t>
+  </si>
+  <si>
+    <t>fflush(stdout</t>
+  </si>
+  <si>
+    <t>//fflush(stdout</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -574,18 +574,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -607,62 +607,62 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -684,62 +684,62 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional rows added to ToInitialize.xlsx
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFE36F0-5014-4E69-9F27-502DB6B502A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3F16AB-076F-4869-8C41-CF945B894F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>FSRcore.c</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>//fflush(stdout</t>
+  </si>
+  <si>
+    <t>double detpar</t>
+  </si>
+  <si>
+    <t>double rotpar=0;</t>
+  </si>
+  <si>
+    <t>double detpar=0;</t>
+  </si>
+  <si>
+    <t>double rotpar</t>
+  </si>
+  <si>
+    <t>double shapepar</t>
+  </si>
+  <si>
+    <t>double shapepar=0;</t>
   </si>
 </sst>
 </file>
@@ -493,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,18 +745,51 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
       <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>32</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added additional items in ToInitialize.xlsx
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279E8E9D-A847-4458-A71A-97F653D193D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B215E7B-CDF7-4783-9D4C-889063A55B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
   <si>
     <t>FSRcore.c</t>
   </si>
@@ -141,19 +141,148 @@
     <t>double detpar</t>
   </si>
   <si>
-    <t>double rotpar=0;</t>
-  </si>
-  <si>
-    <t>double detpar=0;</t>
-  </si>
-  <si>
     <t>double rotpar</t>
   </si>
   <si>
     <t>double shapepar</t>
   </si>
   <si>
-    <t>double shapepar=0;</t>
+    <t>HArho.c</t>
+  </si>
+  <si>
+    <t>double c_data=0</t>
+  </si>
+  <si>
+    <t>double b_data=0</t>
+  </si>
+  <si>
+    <t>double a_data</t>
+  </si>
+  <si>
+    <t>double a_data=0</t>
+  </si>
+  <si>
+    <t>MMregcore.c</t>
+  </si>
+  <si>
+    <t>double A2</t>
+  </si>
+  <si>
+    <t>double A2=0</t>
+  </si>
+  <si>
+    <t>Mscale.c</t>
+  </si>
+  <si>
+    <t>OPTwei.c</t>
+  </si>
+  <si>
+    <t>Sreg.c</t>
+  </si>
+  <si>
+    <t>double scaletest</t>
+  </si>
+  <si>
+    <t>double kc</t>
+  </si>
+  <si>
+    <t>double kc=0</t>
+  </si>
+  <si>
+    <t>double scaletest=0</t>
+  </si>
+  <si>
+    <t>double A</t>
+  </si>
+  <si>
+    <t>double B</t>
+  </si>
+  <si>
+    <t>double d</t>
+  </si>
+  <si>
+    <t>double detpar=0</t>
+  </si>
+  <si>
+    <t>double rotpar=0</t>
+  </si>
+  <si>
+    <t>double shapepar=0</t>
+  </si>
+  <si>
+    <t>double A=0</t>
+  </si>
+  <si>
+    <t>double d=0</t>
+  </si>
+  <si>
+    <t>Sreg_wrapper.c</t>
+  </si>
+  <si>
+    <t>double B=0</t>
+  </si>
+  <si>
+    <t>double c_data</t>
+  </si>
+  <si>
+    <t>double b_data</t>
+  </si>
+  <si>
+    <t>double a2</t>
+  </si>
+  <si>
+    <t>double a2=0</t>
+  </si>
+  <si>
+    <t>double scnew</t>
+  </si>
+  <si>
+    <t>double scnew=0</t>
+  </si>
+  <si>
+    <t>double scaletest</t>
+  </si>
+  <si>
+    <t>double scaletest=0</t>
+  </si>
+  <si>
+    <t>double x1_data</t>
+  </si>
+  <si>
+    <t>double x1_data=0</t>
+  </si>
+  <si>
+    <t>HAwei.c</t>
+  </si>
+  <si>
+    <t>double c2;</t>
+  </si>
+  <si>
+    <t>double c2=0;</t>
+  </si>
+  <si>
+    <t>double b2;</t>
+  </si>
+  <si>
+    <t>double b2=0;</t>
+  </si>
+  <si>
+    <t>double c;</t>
+  </si>
+  <si>
+    <t>double c=0;</t>
+  </si>
+  <si>
+    <t>double c_data;</t>
+  </si>
+  <si>
+    <t>double c_data=0;</t>
+  </si>
+  <si>
+    <t>double b_data=0;</t>
+  </si>
+  <si>
+    <t>double b_data;</t>
   </si>
 </sst>
 </file>
@@ -511,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,7 +881,7 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -760,10 +889,10 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -771,26 +900,246 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
         <v>38</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>16</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>32</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C43" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Regenerated code using precalculated values of bdp and eff for hyperbolic tanngent estimator
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B215E7B-CDF7-4783-9D4C-889063A55B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7E04B0-D128-4AAD-BF97-984EAD17056D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
   <si>
     <t>FSRcore.c</t>
   </si>
@@ -165,12 +165,6 @@
     <t>MMregcore.c</t>
   </si>
   <si>
-    <t>double A2</t>
-  </si>
-  <si>
-    <t>double A2=0</t>
-  </si>
-  <si>
     <t>Mscale.c</t>
   </si>
   <si>
@@ -192,15 +186,6 @@
     <t>double scaletest=0</t>
   </si>
   <si>
-    <t>double A</t>
-  </si>
-  <si>
-    <t>double B</t>
-  </si>
-  <si>
-    <t>double d</t>
-  </si>
-  <si>
     <t>double detpar=0</t>
   </si>
   <si>
@@ -210,30 +195,15 @@
     <t>double shapepar=0</t>
   </si>
   <si>
-    <t>double A=0</t>
-  </si>
-  <si>
-    <t>double d=0</t>
-  </si>
-  <si>
     <t>Sreg_wrapper.c</t>
   </si>
   <si>
-    <t>double B=0</t>
-  </si>
-  <si>
     <t>double c_data</t>
   </si>
   <si>
     <t>double b_data</t>
   </si>
   <si>
-    <t>double a2</t>
-  </si>
-  <si>
-    <t>double a2=0</t>
-  </si>
-  <si>
     <t>double scnew</t>
   </si>
   <si>
@@ -283,6 +253,48 @@
   </si>
   <si>
     <t>double b_data;</t>
+  </si>
+  <si>
+    <t>double d;</t>
+  </si>
+  <si>
+    <t>double d=0;</t>
+  </si>
+  <si>
+    <t>double A2;</t>
+  </si>
+  <si>
+    <t>double A2=0;</t>
+  </si>
+  <si>
+    <t>double ctun;</t>
+  </si>
+  <si>
+    <t>double ctun=0;</t>
+  </si>
+  <si>
+    <t>double B2;</t>
+  </si>
+  <si>
+    <t>double B2=0;</t>
+  </si>
+  <si>
+    <t>double A;</t>
+  </si>
+  <si>
+    <t>double B;</t>
+  </si>
+  <si>
+    <t>double B=0;</t>
+  </si>
+  <si>
+    <t>double A=0;</t>
+  </si>
+  <si>
+    <t>double a2;</t>
+  </si>
+  <si>
+    <t>double a2=0;</t>
   </si>
 </sst>
 </file>
@@ -640,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +893,7 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -892,7 +904,7 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -903,7 +915,7 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -911,7 +923,7 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -922,7 +934,7 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
@@ -944,10 +956,10 @@
         <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -955,10 +967,10 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -966,10 +978,10 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -977,169 +989,224 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
         <v>47</v>
       </c>
-      <c r="B36" t="s">
-        <v>77</v>
-      </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>53</v>
       </c>
-      <c r="C41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C44" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" t="s">
         <v>72</v>
       </c>
-      <c r="B45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" t="s">
-        <v>81</v>
+      <c r="C50" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Everything regenerated with the addition of Sregeda and MMregeda
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7E04B0-D128-4AAD-BF97-984EAD17056D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8314219D-C403-4AA9-B869-991DA43153C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="80">
   <si>
     <t>FSRcore.c</t>
   </si>
@@ -147,30 +147,12 @@
     <t>double shapepar</t>
   </si>
   <si>
-    <t>HArho.c</t>
-  </si>
-  <si>
-    <t>double c_data=0</t>
-  </si>
-  <si>
-    <t>double b_data=0</t>
-  </si>
-  <si>
-    <t>double a_data</t>
-  </si>
-  <si>
-    <t>double a_data=0</t>
-  </si>
-  <si>
     <t>MMregcore.c</t>
   </si>
   <si>
     <t>Mscale.c</t>
   </si>
   <si>
-    <t>OPTwei.c</t>
-  </si>
-  <si>
     <t>Sreg.c</t>
   </si>
   <si>
@@ -198,12 +180,6 @@
     <t>Sreg_wrapper.c</t>
   </si>
   <si>
-    <t>double c_data</t>
-  </si>
-  <si>
-    <t>double b_data</t>
-  </si>
-  <si>
     <t>double scnew</t>
   </si>
   <si>
@@ -216,45 +192,18 @@
     <t>double scaletest=0</t>
   </si>
   <si>
-    <t>double x1_data</t>
-  </si>
-  <si>
-    <t>double x1_data=0</t>
-  </si>
-  <si>
-    <t>HAwei.c</t>
-  </si>
-  <si>
     <t>double c2;</t>
   </si>
   <si>
     <t>double c2=0;</t>
   </si>
   <si>
-    <t>double b2;</t>
-  </si>
-  <si>
-    <t>double b2=0;</t>
-  </si>
-  <si>
     <t>double c;</t>
   </si>
   <si>
     <t>double c=0;</t>
   </si>
   <si>
-    <t>double c_data;</t>
-  </si>
-  <si>
-    <t>double c_data=0;</t>
-  </si>
-  <si>
-    <t>double b_data=0;</t>
-  </si>
-  <si>
-    <t>double b_data;</t>
-  </si>
-  <si>
     <t>double d;</t>
   </si>
   <si>
@@ -267,12 +216,6 @@
     <t>double A2=0;</t>
   </si>
   <si>
-    <t>double ctun;</t>
-  </si>
-  <si>
-    <t>double ctun=0;</t>
-  </si>
-  <si>
     <t>double B2;</t>
   </si>
   <si>
@@ -291,10 +234,46 @@
     <t>double A=0;</t>
   </si>
   <si>
-    <t>double a2;</t>
-  </si>
-  <si>
-    <t>double a2=0;</t>
+    <t>MMreg_wrapper.c</t>
+  </si>
+  <si>
+    <t>double d2;</t>
+  </si>
+  <si>
+    <t>double d2=0;</t>
+  </si>
+  <si>
+    <t>double B2;</t>
+  </si>
+  <si>
+    <t>double B2=0;</t>
+  </si>
+  <si>
+    <t>double A2;</t>
+  </si>
+  <si>
+    <t>double A2=0;</t>
+  </si>
+  <si>
+    <t>int psifunc_class_size_idx_1;</t>
+  </si>
+  <si>
+    <t>int psifunc_class_size_idx_1=1;</t>
+  </si>
+  <si>
+    <t>Sregeda_wrapper.c</t>
+  </si>
+  <si>
+    <t>double scaletest;</t>
+  </si>
+  <si>
+    <t>double scaletest=1;</t>
+  </si>
+  <si>
+    <t>double psifunc_kc1;</t>
+  </si>
+  <si>
+    <t>double psifunc_kc1=0;</t>
   </si>
 </sst>
 </file>
@@ -652,16 +631,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -893,7 +872,7 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,7 +883,7 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,7 +894,7 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -923,10 +902,10 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -934,10 +913,10 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -945,81 +924,81 @@
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
         <v>42</v>
-      </c>
-      <c r="B29" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>56</v>
@@ -1030,139 +1009,133 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>53</v>
-      </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
         <v>53</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
         <v>73</v>
@@ -1172,41 +1145,91 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" t="s">
         <v>62</v>
       </c>
-      <c r="B50" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" t="s">
-        <v>71</v>
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fsdaC regenerated with setdiffFS and [2,4,8] changed with [2;4;8]
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8314219D-C403-4AA9-B869-991DA43153C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22067D3-F9C2-456E-9E72-291615B6FF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
   <si>
     <t>FSRcore.c</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>double psifunc_kc1=0;</t>
+  </si>
+  <si>
+    <t>MMregeda_wrapper.c</t>
   </si>
 </sst>
 </file>
@@ -631,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,6 +1235,50 @@
         <v>57</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LIbrary regenerated with tuning parameters as column vectors. Updated test files and ToInitialize.xlsx
</commit_message>
<xml_diff>
--- a/wrapper/ToInitialize.xlsx
+++ b/wrapper/ToInitialize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA-MATLAB_Coder\wrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22067D3-F9C2-456E-9E72-291615B6FF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0B7DCE-4B83-470D-8725-78E9AFA68258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07DE166B-144F-43CB-9C7B-5D03E3821701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="83">
   <si>
     <t>FSRcore.c</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>MMregeda_wrapper.c</t>
+  </si>
+  <si>
+    <t>double b_c;</t>
+  </si>
+  <si>
+    <t>double b_c=0;</t>
   </si>
 </sst>
 </file>
@@ -634,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDC7D5-A18A-40F5-9A02-1CA2A81399AF}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1237,13 +1243,13 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C55" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1251,10 +1257,10 @@
         <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1262,10 +1268,10 @@
         <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1273,9 +1279,20 @@
         <v>80</v>
       </c>
       <c r="B58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" t="s">
         <v>71</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>